<commit_message>
fix E of woods
</commit_message>
<xml_diff>
--- a/structures/material_properties.xlsx
+++ b/structures/material_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365.sharepoint.com/sites/DSEGroup18-WingsforAid/Gedeelde documenten/DID-07 Midterm/Analysis/Material selection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janvonken/Desktop/TU/3rd Year/DSE/WingsForAid/structures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1172" documentId="11_5863A68DEB42F1A67B902BE7F639F66872003D32" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F56D3471-1CC0-43C0-B4DB-2EB8270C965F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00C4AAF-6ED1-FB46-B366-03FD23AF108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -691,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -714,15 +714,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -730,6 +722,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1060,36 +1055,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H45"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="8" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:17">
       <c r="C2" s="1" t="s">
@@ -1113,7 +1108,7 @@
       <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1478,7 +1473,7 @@
       <c r="C13">
         <v>2850</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13">
         <v>10.130000000000001</v>
       </c>
       <c r="E13">
@@ -1577,7 +1572,7 @@
         <f>A14+1</f>
         <v>9</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C17">
@@ -1628,7 +1623,7 @@
         <f>A17+1</f>
         <v>10</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C18">
@@ -1679,7 +1674,7 @@
         <f t="shared" ref="A19:A24" si="3">A18+1</f>
         <v>11</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C19">
@@ -1730,7 +1725,7 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C20">
@@ -1781,7 +1776,7 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C21">
@@ -1832,7 +1827,7 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C22">
@@ -1883,7 +1878,7 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C23">
@@ -1934,7 +1929,7 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="14" t="s">
         <v>79</v>
       </c>
       <c r="C24">
@@ -1989,7 +1984,7 @@
       <c r="A27">
         <v>17</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>84</v>
       </c>
       <c r="C27">
@@ -2040,7 +2035,7 @@
       <c r="A28">
         <v>18</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C28">
@@ -2096,7 +2091,7 @@
         <f>A28+1</f>
         <v>19</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C31">
@@ -2147,7 +2142,7 @@
         <f>A31+1</f>
         <v>20</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>96</v>
       </c>
       <c r="C32">
@@ -2193,12 +2188,12 @@
         <v>581.94888091652854</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:17">
       <c r="B34" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:17">
       <c r="A35">
         <f>A32+1</f>
         <v>21</v>
@@ -2251,7 +2246,7 @@
         <v>414.90751453069043</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:17">
       <c r="A36">
         <f>A35+1</f>
         <v>22</v>
@@ -2262,7 +2257,7 @@
       <c r="C36">
         <v>4650</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="12">
         <v>30</v>
       </c>
       <c r="E36">
@@ -2304,9 +2299,9 @@
         <v>435.51240238548769</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:17">
       <c r="A37">
-        <f t="shared" ref="A37:A40" si="4">A36+1</f>
+        <f t="shared" ref="A37:A39" si="4">A36+1</f>
         <v>23</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -2357,7 +2352,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:17">
       <c r="A38">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -2368,7 +2363,7 @@
       <c r="C38">
         <v>4650</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="12">
         <v>30</v>
       </c>
       <c r="E38">
@@ -2410,7 +2405,7 @@
         <v>443.36010399920042</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:17">
       <c r="A39">
         <f t="shared" si="4"/>
         <v>25</v>
@@ -2421,7 +2416,7 @@
       <c r="C39">
         <v>4780</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="12">
         <v>25</v>
       </c>
       <c r="E39">
@@ -2460,15 +2455,15 @@
         <v>527.86269463776648</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:17">
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:17">
       <c r="B41" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:17">
       <c r="A42">
         <f>A39+1</f>
         <v>26</v>
@@ -2509,52 +2504,45 @@
         <v>147.78670133306682</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
-      <c r="A43" s="11">
+    <row r="43" spans="1:17">
+      <c r="A43">
         <f>A42+1</f>
         <v>27</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43">
         <v>1438</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="12">
         <v>30</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43">
         <v>3.92</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43">
         <v>4.12</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43">
         <v>170</v>
       </c>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11">
+      <c r="I43">
         <v>110</v>
       </c>
-      <c r="J43" s="14"/>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11">
+      <c r="P43">
         <f>C43/G43</f>
         <v>8.4588235294117649</v>
       </c>
-      <c r="Q43" s="11">
+      <c r="Q43">
         <f>C43/SQRT(I43)</f>
         <v>137.10792033351618</v>
       </c>
-      <c r="R43" s="11"/>
-    </row>
-    <row r="44" spans="1:18" s="11" customFormat="1">
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <f t="shared" ref="A44:A46" si="5">A43+1</f>
         <v>28</v>
@@ -2577,20 +2565,15 @@
       <c r="G44">
         <v>150</v>
       </c>
-      <c r="H44"/>
       <c r="I44">
         <v>22</v>
       </c>
       <c r="J44" s="8">
         <v>15</v>
       </c>
-      <c r="K44"/>
-      <c r="L44"/>
       <c r="M44" t="s">
         <v>73</v>
       </c>
-      <c r="N44"/>
-      <c r="O44"/>
       <c r="P44">
         <f>C44/G44</f>
         <v>12.666666666666666</v>
@@ -2599,9 +2582,8 @@
         <f>C44/SQRT(I44)</f>
         <v>405.0813610756598</v>
       </c>
-      <c r="R44"/>
-    </row>
-    <row r="45" spans="1:18" ht="152.25">
+    </row>
+    <row r="45" spans="1:17" ht="128">
       <c r="A45">
         <f t="shared" si="5"/>
         <v>29</v>
@@ -2650,7 +2632,7 @@
         <v>321.42379036413621</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="16.5" customHeight="1">
+    <row r="46" spans="1:17" ht="16.5" customHeight="1">
       <c r="A46">
         <f t="shared" si="5"/>
         <v>30</v>
@@ -2661,13 +2643,13 @@
       <c r="C46">
         <v>2450</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46">
         <v>15</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E46" s="12">
         <v>4</v>
       </c>
-      <c r="F46" s="16">
+      <c r="F46" s="12">
         <v>20</v>
       </c>
       <c r="G46">
@@ -2688,7 +2670,7 @@
         <v>292.83100928692642</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:17">
       <c r="B48" s="2" t="s">
         <v>128</v>
       </c>
@@ -2733,11 +2715,11 @@
         <v>73</v>
       </c>
       <c r="P49">
-        <f>C49/G49</f>
+        <f t="shared" ref="P49:P57" si="6">C49/G49</f>
         <v>18.888888888888889</v>
       </c>
       <c r="Q49">
-        <f>C49/SQRT(I49)</f>
+        <f t="shared" ref="Q49:Q57" si="7">C49/SQRT(I49)</f>
         <v>687.04682033565473</v>
       </c>
     </row>
@@ -2755,7 +2737,7 @@
       <c r="D50">
         <v>4.3</v>
       </c>
-      <c r="E50" s="16">
+      <c r="E50" s="12">
         <v>1.4</v>
       </c>
       <c r="F50" s="8">
@@ -2781,17 +2763,17 @@
         <v>73</v>
       </c>
       <c r="P50">
-        <f>C50/G50</f>
+        <f t="shared" si="6"/>
         <v>15.479452054794521</v>
       </c>
       <c r="Q50">
-        <f>C50/SQRT(I50)</f>
+        <f t="shared" si="7"/>
         <v>663.55884805161497</v>
       </c>
     </row>
     <row r="51" spans="1:17">
       <c r="A51">
-        <f t="shared" ref="A51:A56" si="6">A50+1</f>
+        <f t="shared" ref="A51:A56" si="8">A50+1</f>
         <v>33</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -2829,17 +2811,17 @@
         <v>73</v>
       </c>
       <c r="P51">
-        <f>C51/G51</f>
+        <f t="shared" si="6"/>
         <v>17.692307692307693</v>
       </c>
       <c r="Q51">
-        <f>C51/SQRT(I51)</f>
+        <f t="shared" si="7"/>
         <v>775.32984183272833</v>
       </c>
     </row>
     <row r="52" spans="1:17">
       <c r="A52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -2876,17 +2858,17 @@
         <v>73</v>
       </c>
       <c r="P52">
-        <f>C52/G52</f>
+        <f t="shared" si="6"/>
         <v>31.428571428571427</v>
       </c>
       <c r="Q52">
-        <f>C52/SQRT(I52)</f>
+        <f t="shared" si="7"/>
         <v>777.81745930520219</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -2924,17 +2906,17 @@
         <v>73</v>
       </c>
       <c r="P53">
-        <f>C53/G53</f>
+        <f t="shared" si="6"/>
         <v>107.5</v>
       </c>
       <c r="Q53">
-        <f>C53/SQRT(I53)</f>
+        <f t="shared" si="7"/>
         <v>3040.5591591021544</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2971,17 +2953,17 @@
         <v>73</v>
       </c>
       <c r="P54">
-        <f>C54/G54</f>
+        <f t="shared" si="6"/>
         <v>16.375</v>
       </c>
       <c r="Q54">
-        <f>C54/SQRT(I54)</f>
+        <f t="shared" si="7"/>
         <v>663.34428543980164</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -3018,17 +3000,17 @@
         <v>73</v>
       </c>
       <c r="P55">
-        <f>C55/G55</f>
+        <f t="shared" si="6"/>
         <v>33.333333333333336</v>
       </c>
       <c r="Q55">
-        <f>C55/SQRT(I55)</f>
+        <f t="shared" si="7"/>
         <v>823.54465965824397</v>
       </c>
     </row>
     <row r="56" spans="1:17">
       <c r="A56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -3065,11 +3047,11 @@
         <v>73</v>
       </c>
       <c r="P56">
-        <f>C56/G56</f>
+        <f t="shared" si="6"/>
         <v>31.03448275862069</v>
       </c>
       <c r="Q56">
-        <f>C56/SQRT(I56)</f>
+        <f t="shared" si="7"/>
         <v>789.35221737632628</v>
       </c>
     </row>
@@ -3112,11 +3094,11 @@
         <v>73</v>
       </c>
       <c r="P57">
-        <f>C57/G57</f>
+        <f t="shared" si="6"/>
         <v>40.425531914893618</v>
       </c>
       <c r="Q57">
-        <f>C57/SQRT(I57)</f>
+        <f t="shared" si="7"/>
         <v>1062.1322893124002</v>
       </c>
     </row>
@@ -3149,7 +3131,7 @@
         <v>20.7</v>
       </c>
       <c r="I60">
-        <v>7.0000000000000007E-2</v>
+        <v>8.14</v>
       </c>
       <c r="J60" s="8">
         <v>7</v>
@@ -3169,7 +3151,7 @@
       </c>
       <c r="Q60">
         <f>C60/SQRT(I60)</f>
-        <v>1285.0792082313724</v>
+        <v>119.16993832957286</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -3221,7 +3203,7 @@
     </row>
     <row r="62" spans="1:17">
       <c r="A62">
-        <f t="shared" ref="A62:A63" si="7">A61+1</f>
+        <f t="shared" ref="A62:A63" si="9">A61+1</f>
         <v>42</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -3243,7 +3225,7 @@
         <v>34</v>
       </c>
       <c r="I62">
-        <v>0.06</v>
+        <v>9.31</v>
       </c>
       <c r="J62" s="8">
         <v>7</v>
@@ -3263,12 +3245,12 @@
       </c>
       <c r="Q62">
         <f>C62/SQRT(I62)</f>
-        <v>2245.3655975512465</v>
+        <v>180.25521946972711</v>
       </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -3290,7 +3272,7 @@
         <v>34.5</v>
       </c>
       <c r="I63">
-        <v>0.05</v>
+        <v>10.9</v>
       </c>
       <c r="J63" s="8">
         <v>6</v>
@@ -3307,7 +3289,7 @@
       </c>
       <c r="Q63">
         <f>C63/SQRT(I63)</f>
-        <v>2012.4611797498108</v>
+        <v>136.30106988346111</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -3456,11 +3438,11 @@
         <v>130</v>
       </c>
       <c r="P71">
-        <f t="shared" ref="P71:P77" si="8">C71/G71</f>
+        <f t="shared" ref="P71:P77" si="10">C71/G71</f>
         <v>7.8723404255319149</v>
       </c>
       <c r="Q71">
-        <f t="shared" ref="Q71:Q77" si="9">C71/SQRT(I71)</f>
+        <f t="shared" ref="Q71:Q77" si="11">C71/SQRT(I71)</f>
         <v>277.32672492846871</v>
       </c>
     </row>
@@ -3511,11 +3493,11 @@
         <v>73</v>
       </c>
       <c r="P74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>23.707865168539325</v>
       </c>
       <c r="Q74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>409.11145235880139</v>
       </c>
     </row>
@@ -3558,11 +3540,11 @@
         <v>73</v>
       </c>
       <c r="P75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10.138461538461538</v>
       </c>
       <c r="Q75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>182.773714656213</v>
       </c>
     </row>
@@ -3605,11 +3587,11 @@
         <v>73</v>
       </c>
       <c r="P76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.359223300970875</v>
       </c>
       <c r="Q76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>261.09196480264774</v>
       </c>
     </row>
@@ -3652,11 +3634,11 @@
         <v>73</v>
       </c>
       <c r="P77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.2376237623762378</v>
       </c>
       <c r="Q77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>151.90648898367982</v>
       </c>
     </row>
@@ -3670,7 +3652,7 @@
       </c>
       <c r="Q79">
         <f>MIN(Q7:Q77)</f>
-        <v>137.10792033351618</v>
+        <v>119.16993832957286</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -3779,20 +3761,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DBB733-8FA8-49ED-BB9F-0430831C7787}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5165,7 +5147,7 @@
       </c>
       <c r="G41">
         <f>Sheet1!I60</f>
-        <v>7.0000000000000007E-2</v>
+        <v>8.14</v>
       </c>
       <c r="H41">
         <f>Sheet1!J60</f>
@@ -5233,7 +5215,7 @@
       </c>
       <c r="G43">
         <f>Sheet1!I62</f>
-        <v>0.06</v>
+        <v>9.31</v>
       </c>
       <c r="H43">
         <f>Sheet1!J62</f>
@@ -5267,7 +5249,7 @@
       </c>
       <c r="G44">
         <f>Sheet1!I63</f>
-        <v>0.05</v>
+        <v>10.9</v>
       </c>
       <c r="H44">
         <f>Sheet1!J63</f>
@@ -5518,12 +5500,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="46afbdc8-40ba-417d-b3e9-facef3290d04" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f525c1f-400e-47f8-8a8b-5e89483b5ff6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5722,24 +5706,48 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="46afbdc8-40ba-417d-b3e9-facef3290d04" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f525c1f-400e-47f8-8a8b-5e89483b5ff6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC46062-5973-4779-AB8C-CA727C413686}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785DBE7F-03A2-4811-BB48-4CC5E2E607F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46afbdc8-40ba-417d-b3e9-facef3290d04"/>
+    <ds:schemaRef ds:uri="1f525c1f-400e-47f8-8a8b-5e89483b5ff6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{222DE826-ACCC-4E24-AE0D-A4319801D8FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{222DE826-ACCC-4E24-AE0D-A4319801D8FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1f525c1f-400e-47f8-8a8b-5e89483b5ff6"/>
+    <ds:schemaRef ds:uri="46afbdc8-40ba-417d-b3e9-facef3290d04"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785DBE7F-03A2-4811-BB48-4CC5E2E607F1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC46062-5973-4779-AB8C-CA727C413686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>